<commit_message>
School data Analysis with Pandas updates
</commit_message>
<xml_diff>
--- a/school_district_analysis.xlsx
+++ b/school_district_analysis.xlsx
@@ -444,42 +444,42 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Total schools</t>
+          <t>Total Schools</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Total students</t>
+          <t>Total Students</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total budget</t>
+          <t>Total Budget</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Average math score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Average reading score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% passing math</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>% passing reading</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>% overall passing</t>
+          <t>% Overall Passing</t>
         </is>
       </c>
     </row>
@@ -541,32 +541,32 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total budget</t>
+          <t>Total Budget</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Average math score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Average reading score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% passing math</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>% passing reading</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>% Overall passing</t>
+          <t>% Overall Passing</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -1182,32 +1182,32 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total budget</t>
+          <t>Total Budget</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Average math score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Average reading score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% passing math</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>% passing reading</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>% Overall passing</t>
+          <t>% Overall Passing</t>
         </is>
       </c>
     </row>
@@ -1383,32 +1383,32 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total budget</t>
+          <t>Total Budget</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Average math score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Average reading score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% passing math</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>% passing reading</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>% Overall passing</t>
+          <t>% Overall Passing</t>
         </is>
       </c>
     </row>
@@ -2241,27 +2241,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Average math score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Average reading score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>% passing math</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>% passing reading</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% Overall passing</t>
+          <t>% Overall Passing</t>
         </is>
       </c>
     </row>
@@ -2380,27 +2380,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Average math score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Average reading score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>% passing math</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>% passing reading</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% Overall passing</t>
+          <t>% Overall Passing</t>
         </is>
       </c>
     </row>
@@ -2497,27 +2497,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Average math score</t>
+          <t>Average Math Score</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Average reading score</t>
+          <t>Average Reading Score</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>% passing math</t>
+          <t>% Passing Math</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>% passing reading</t>
+          <t>% Passing Reading</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% Overall passing</t>
+          <t>% Overall Passing</t>
         </is>
       </c>
     </row>

</xml_diff>